<commit_message>
updated commit on 10 march 2024
</commit_message>
<xml_diff>
--- a/Test_Data/read.xlsx
+++ b/Test_Data/read.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nine\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nine\eclipse-workspace\Selenium_java_2023\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8385F9BD-6975-4C19-8F4B-33022E7E4E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D822F5CC-FF8A-4DBB-9B71-00013A1D66C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Pince</t>
   </si>
   <si>
-    <t>Qualification</t>
-  </si>
-  <si>
     <t>Mtech</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>2nd std</t>
+  </si>
+  <si>
+    <t>Quali.</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +418,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -432,7 +432,7 @@
         <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>0.67</v>
@@ -446,7 +446,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>0.78</v>
@@ -460,7 +460,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>0.55000000000000004</v>
@@ -474,7 +474,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>0.89</v>

</xml_diff>